<commit_message>
Implement Enum Class in TypeScript.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgEnumValueObject.xlsx
+++ b/meta/program/BlancoCgEnumValueObject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{76419C30-5BEE-D54F-84F1-29A0D54A2479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C968D09-BD77-514A-AF89-B21C4FC32D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -272,13 +272,34 @@
     <rPh sb="52" eb="55">
       <t>ミタイオウ</t>
     </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>java.lang.Boolean</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>クラス内定義など必要に応じてLineTerminatorを付与します。</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">ヒツヨウニ </t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t xml:space="preserve">オウジテ </t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t xml:space="preserve">フヨシマス </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>lineTerminator</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -814,6 +835,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -833,18 +866,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1245,13 +1266,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -1317,12 +1340,12 @@
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="52"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="56"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
@@ -1423,23 +1446,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="54"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="58"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="56"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="54"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="58"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -1476,29 +1499,29 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E25" s="49" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="56"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6">
@@ -1546,10 +1569,10 @@
         <v>33</v>
       </c>
       <c r="D29" s="46"/>
-      <c r="E29" s="53" t="s">
+      <c r="E29" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="49"/>
+      <c r="F29" s="53"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="44">
@@ -1565,19 +1588,27 @@
       <c r="D30" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="53" t="s">
+      <c r="E30" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="49"/>
+      <c r="F30" s="53"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="44">
         <v>5</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
+      <c r="B31" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="46" t="s">
+        <v>49</v>
+      </c>
       <c r="F31" s="47"/>
     </row>
     <row r="32" spans="1:6" ht="82.5" customHeight="1">
@@ -1591,10 +1622,10 @@
         <v>45</v>
       </c>
       <c r="D32" s="24"/>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="49"/>
+      <c r="F32" s="53"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="22"/>
@@ -1614,6 +1645,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
@@ -1622,32 +1659,26 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D50">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D50" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>
@@ -1660,7 +1691,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
2.3.17: Available Enum class expand for TypeScript and Kotlin.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgEnumValueObject.xlsx
+++ b/meta/program/BlancoCgEnumValueObject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C968D09-BD77-514A-AF89-B21C4FC32D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32998D6-F9D6-5B4D-A7FF-560C0FAD765C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -294,13 +294,41 @@
   <si>
     <t>lineTerminator</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>constructorArgList</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>java.util.List&lt;blanco.cg.valueobject.BlancoCgField&gt;</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>new java.util.ArrayList&lt;blanco.cg.valueobject.BlancoCgField&gt;()</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>クラス定義に含めるコンストラクタの引数マップです。&lt;引数名, 型&gt; となります。</t>
+    <rPh sb="6" eb="7">
+      <t xml:space="preserve">フクメル </t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">ヒキスウ </t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t xml:space="preserve">ヒキスウメイ </t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t xml:space="preserve">カタ </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -330,6 +358,18 @@
       <name val="ＭＳ ゴシック"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -710,7 +750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -759,9 +799,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -835,38 +872,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1270,10 +1316,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1289,7 +1335,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="32" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1340,19 +1386,19 @@
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="D9"/>
@@ -1364,7 +1410,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="37"/>
+      <c r="C10" s="36"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
@@ -1374,7 +1420,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="36" t="s">
         <v>17</v>
       </c>
       <c r="D11"/>
@@ -1386,7 +1432,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>17</v>
       </c>
       <c r="D12"/>
@@ -1398,7 +1444,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="37"/>
+      <c r="C13" s="36"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -1432,8 +1478,8 @@
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
@@ -1446,39 +1492,39 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="58"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="53"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="48"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="58"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="53"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="18"/>
       <c r="B21" s="20"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="41"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="40"/>
       <c r="F21"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="26"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="42"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="41"/>
       <c r="F22"/>
     </row>
     <row r="23" spans="1:6">
@@ -1499,29 +1545,29 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="49" t="s">
+      <c r="E25" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="30"/>
+      <c r="F25" s="29"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6">
@@ -1541,116 +1587,132 @@
       <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="44">
+      <c r="A28" s="43">
         <f>A27+1</f>
         <v>2</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46" t="s">
+      <c r="D28" s="45"/>
+      <c r="E28" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="47"/>
+      <c r="F28" s="46"/>
     </row>
     <row r="29" spans="1:6" ht="31.5" customHeight="1">
-      <c r="A29" s="44">
-        <f>A28+1</f>
+      <c r="A29" s="43">
+        <f t="shared" ref="A29:A33" si="0">A28+1</f>
         <v>3</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="46"/>
-      <c r="E29" s="57" t="s">
+      <c r="D29" s="45"/>
+      <c r="E29" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="53"/>
+      <c r="F29" s="48"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="44">
-        <f>A29+1</f>
+      <c r="A30" s="43">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="46" t="s">
+      <c r="D30" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="57" t="s">
+      <c r="E30" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="53"/>
+      <c r="F30" s="48"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="44">
+      <c r="A31" s="43">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="46" t="b">
+      <c r="D31" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="47"/>
+      <c r="F31" s="46"/>
     </row>
     <row r="32" spans="1:6" ht="82.5" customHeight="1">
-      <c r="A32" s="44">
+      <c r="A32" s="43">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="52" t="s">
+      <c r="D32" s="23"/>
+      <c r="E32" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="22"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="25"/>
+      <c r="A33" s="43">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B33" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="48"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="26"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="29"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="24"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
+  <mergeCells count="15">
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
@@ -1659,10 +1721,16 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D50" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D51" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1724,54 +1792,54 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="33"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="35" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="38"/>
-      <c r="D4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="B4" s="37"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="35" t="s">
+      <c r="J5" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="40"/>
+      <c r="B6" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>

<commit_message>
2.3.18: Improvement enumeration class: enable constructor.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgEnumValueObject.xlsx
+++ b/meta/program/BlancoCgEnumValueObject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32998D6-F9D6-5B4D-A7FF-560C0FAD765C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215BC9A4-296D-C441-865E-1D05739E4746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18800" yWindow="1680" windowWidth="25840" windowHeight="21100" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -322,6 +322,20 @@
       <t xml:space="preserve">カタ </t>
     </rPh>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>methodList</t>
+  </si>
+  <si>
+    <t>java.util.List&lt;blanco.cg.valueobject.BlancoCgMethod&gt;</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>new java.util.ArrayList&lt;blanco.cg.valueobject.BlancoCgMethod&gt;()</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>このクラスに含まれるメソッドのリストです。</t>
   </si>
 </sst>
 </file>
@@ -872,12 +886,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -892,27 +927,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1316,10 +1330,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1386,12 +1400,12 @@
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="58"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
@@ -1492,23 +1506,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="60"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="55"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="53"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="60"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -1545,29 +1559,29 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="52" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="29"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="55"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
+      <c r="A26" s="51"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6">
@@ -1605,7 +1619,7 @@
     </row>
     <row r="29" spans="1:6" ht="31.5" customHeight="1">
       <c r="A29" s="43">
-        <f t="shared" ref="A29:A33" si="0">A28+1</f>
+        <f t="shared" ref="A29:A34" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="44" t="s">
@@ -1615,10 +1629,10 @@
         <v>33</v>
       </c>
       <c r="D29" s="45"/>
-      <c r="E29" s="52" t="s">
+      <c r="E29" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="48"/>
+      <c r="F29" s="50"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="43">
@@ -1634,10 +1648,10 @@
       <c r="D30" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="52" t="s">
+      <c r="E30" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="48"/>
+      <c r="F30" s="50"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="43">
@@ -1670,67 +1684,86 @@
         <v>45</v>
       </c>
       <c r="D32" s="23"/>
-      <c r="E32" s="47" t="s">
+      <c r="E32" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="50"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="43">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="59" t="s">
+      <c r="C33" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="59" t="s">
+      <c r="D33" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="60" t="s">
+      <c r="E33" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="48"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="43"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
+      <c r="F33" s="50"/>
+    </row>
+    <row r="34" spans="1:6" ht="14" customHeight="1">
+      <c r="A34" s="43">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="48" t="s">
+        <v>58</v>
+      </c>
       <c r="F34" s="24"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="25"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="28"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="24"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E33:F33"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D51" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D52" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
3.0.8: [Kotlin] Support annotation for Enum Class.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgEnumValueObject.xlsx
+++ b/meta/program/BlancoCgEnumValueObject.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215BC9A4-296D-C441-865E-1D05739E4746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03316638-14B1-ED46-A4BD-931017606FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18800" yWindow="1680" windowWidth="25840" windowHeight="21100" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -336,6 +336,26 @@
   </si>
   <si>
     <t>このクラスに含まれるメソッドのリストです。</t>
+  </si>
+  <si>
+    <t>annotationList</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>java.util.List&lt;java.lang.String&gt;</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>new java.util.ArrayList&lt;java.lang.String&gt;()</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>new java.util.ArrayList&lt;java.lang.String&gt;()</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>このクラスに付与されているアノテーションのリストです。</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -764,16 +784,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -873,7 +892,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -892,41 +910,41 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1330,10 +1348,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1349,7 +1367,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1372,47 +1390,47 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="58"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="36" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="35" t="s">
         <v>27</v>
       </c>
       <c r="D9"/>
@@ -1420,21 +1438,21 @@
       <c r="F9"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="35"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="36" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="35" t="s">
         <v>17</v>
       </c>
       <c r="D11"/>
@@ -1442,11 +1460,11 @@
       <c r="F11"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="36" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="35" t="s">
         <v>17</v>
       </c>
       <c r="D12"/>
@@ -1454,21 +1472,21 @@
       <c r="F12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="36"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="35"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
@@ -1480,276 +1498,291 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="11"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="6"/>
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="60"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="52"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="51"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="60"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="52"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="18"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="40"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="39"/>
       <c r="F21"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="25"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="41"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="40"/>
       <c r="F22"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="52" t="s">
+      <c r="D25" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="52" t="s">
+      <c r="E25" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="29"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="51"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="9"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="18">
+      <c r="A27" s="17">
         <v>1</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="21"/>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="43">
+      <c r="A28" s="41">
         <f>A27+1</f>
         <v>2</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45" t="s">
+      <c r="D28" s="43"/>
+      <c r="E28" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="46"/>
+      <c r="F28" s="44"/>
     </row>
     <row r="29" spans="1:6" ht="31.5" customHeight="1">
-      <c r="A29" s="43">
-        <f t="shared" ref="A29:A34" si="0">A28+1</f>
+      <c r="A29" s="41">
+        <f t="shared" ref="A29:A35" si="0">A28+1</f>
         <v>3</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="59" t="s">
+      <c r="D29" s="43"/>
+      <c r="E29" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="50"/>
+      <c r="F29" s="51"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="43">
+      <c r="A30" s="41">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="C30" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="D30" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="59" t="s">
+      <c r="E30" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="50"/>
+      <c r="F30" s="51"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="43">
+      <c r="A31" s="41">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="45" t="b">
+      <c r="D31" s="43" t="b">
         <v>0</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="44"/>
     </row>
     <row r="32" spans="1:6" ht="82.5" customHeight="1">
-      <c r="A32" s="43">
+      <c r="A32" s="41">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="55" t="s">
+      <c r="D32" s="22"/>
+      <c r="E32" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="50"/>
+      <c r="F32" s="51"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="43">
+      <c r="A33" s="41">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="48" t="s">
+      <c r="D33" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="50"/>
+      <c r="F33" s="51"/>
     </row>
     <row r="34" spans="1:6" ht="14" customHeight="1">
-      <c r="A34" s="43">
+      <c r="A34" s="41">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="48" t="s">
+      <c r="C34" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="48" t="s">
+      <c r="E34" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="F34" s="24"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="43"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="24"/>
+      <c r="F34" s="23"/>
+    </row>
+    <row r="35" spans="1:6" ht="14" customHeight="1">
+      <c r="A35" s="41">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="25"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="28"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="23"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="24"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
@@ -1759,11 +1792,15 @@
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D52" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D53" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1825,54 +1862,54 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="32"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="37"/>
-      <c r="D4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="36"/>
+      <c r="D4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="39"/>
+      <c r="B6" s="38"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>